<commit_message>
add left/right and modules import
</commit_message>
<xml_diff>
--- a/Excel/TestSheet.xlsx
+++ b/Excel/TestSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crdan_000\Documents\code\html_javascript\frc_scoutingpass_2024\ScoutingPASS\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crdan\Documents\code\javascript\FRC\ScoutingPASS\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C0D11A-B476-4E37-BF18-025A9A5B60BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686FC7EF-4F63-4D7E-BA85-390E80BFDF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29835" yWindow="1125" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="503" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -413,15 +413,15 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,7 +498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
update excel needs, add TBA api key
</commit_message>
<xml_diff>
--- a/Excel/TestSheet.xlsx
+++ b/Excel/TestSheet.xlsx
@@ -5,16 +5,16 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crdan_000\Documents\code\html_javascript\frc_scoutingpass_2024\ScoutingPASS\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crdan\Documents\code\javascript\FRC\ScoutingPASS\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE9689A-ABCF-47DA-9636-F80C4A7C333D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF514AA-7ED7-4B6B-A6D7-9488F4F67656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="463" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="503" windowWidth="22695" windowHeight="14595" tabRatio="463" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="IndividualTeam" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
   <si>
     <t>s</t>
   </si>
@@ -69,18 +69,12 @@
     <t>Match #</t>
   </si>
   <si>
-    <t>CA</t>
-  </si>
-  <si>
     <t>grand forks</t>
   </si>
   <si>
     <t>p</t>
   </si>
   <si>
-    <t>[13]</t>
-  </si>
-  <si>
     <t>l</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>n</t>
   </si>
   <si>
-    <t>com</t>
-  </si>
-  <si>
     <t>Position</t>
   </si>
   <si>
@@ -151,6 +142,81 @@
   </si>
   <si>
     <t>Times Amplified</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>Grand forks</t>
+  </si>
+  <si>
+    <t>qm</t>
+  </si>
+  <si>
+    <t>[48]</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>Talon stinky</t>
+  </si>
+  <si>
+    <t>Bs</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>[37]</t>
+  </si>
+  <si>
+    <t>Carter booty</t>
+  </si>
+  <si>
+    <t>GH</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>test :D</t>
+  </si>
+  <si>
+    <t>Pog</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>r1</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <t>good defense, how many times they were voted good at defense</t>
+  </si>
+  <si>
+    <t>auto, total scores during auto</t>
+  </si>
+  <si>
+    <t>climb, if they climbed in a match succesfully</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>driver skill, same as defense</t>
+  </si>
+  <si>
+    <t>Scores, average</t>
   </si>
 </sst>
 </file>
@@ -199,7 +265,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -312,15 +413,15 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Endgame" pivot="0" count="3" xr9:uid="{38911349-03B7-4372-9916-EB99E6E56839}">
-      <tableStyleElement type="wholeTable" dxfId="7"/>
-      <tableStyleElement type="headerRow" dxfId="6"/>
-      <tableStyleElement type="firstRowStripe" dxfId="5"/>
+      <tableStyleElement type="wholeTable" dxfId="12"/>
+      <tableStyleElement type="headerRow" dxfId="11"/>
+      <tableStyleElement type="firstRowStripe" dxfId="10"/>
     </tableStyle>
     <tableStyle name="Miscellaneous" pivot="0" count="4" xr9:uid="{4C99B414-7197-4D54-A8CA-E08CBAD8C634}">
-      <tableStyleElement type="wholeTable" dxfId="4"/>
-      <tableStyleElement type="headerRow" dxfId="3"/>
-      <tableStyleElement type="firstRowStripe" dxfId="2"/>
-      <tableStyleElement type="secondRowStripe" dxfId="1"/>
+      <tableStyleElement type="wholeTable" dxfId="9"/>
+      <tableStyleElement type="headerRow" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="secondRowStripe" dxfId="6"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -403,11 +504,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>IndividualTeam!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2134</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -426,41 +527,32 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$2:$C$5</c:f>
+              <c:f>IndividualTeam!$C$2:$C$5</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Amp Scores</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Speaker Scores</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Times Amplified</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Pickup From</c:v>
+                  <c:v>Scores, average</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$5</c:f>
+              <c:f>IndividualTeam!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1562,20 +1654,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="9" width="11" customWidth="1"/>
     <col min="10" max="22" width="12" customWidth="1"/>
     <col min="23" max="26" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1595,215 +1687,212 @@
         <v>8</v>
       </c>
       <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="V1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="O1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" t="s">
-        <v>29</v>
-      </c>
-      <c r="U1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" t="s">
-        <v>30</v>
-      </c>
-      <c r="W1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2">
+        <v>246</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="D2">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>2</v>
       </c>
-      <c r="F2">
-        <v>2134</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
       <c r="K2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L2">
         <v>3</v>
       </c>
       <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>6</v>
+      </c>
+      <c r="O2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2">
         <v>4</v>
-      </c>
-      <c r="N2">
-        <v>5</v>
-      </c>
-      <c r="O2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2">
-        <v>5.2</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2" t="s">
-        <v>16</v>
-      </c>
-      <c r="T2" t="s">
-        <v>3</v>
-      </c>
-      <c r="U2">
-        <v>3</v>
       </c>
       <c r="V2">
         <v>0</v>
       </c>
       <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
         <v>0</v>
-      </c>
-      <c r="X2">
-        <v>1</v>
       </c>
       <c r="Y2">
         <v>0</v>
       </c>
-      <c r="Z2" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3">
+        <v>8396</v>
+      </c>
+      <c r="G3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <v>11</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3">
         <v>2</v>
       </c>
-      <c r="F3">
-        <v>2254</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>5</v>
-      </c>
-      <c r="L3">
-        <v>6</v>
-      </c>
-      <c r="M3">
-        <v>7</v>
-      </c>
-      <c r="N3">
-        <v>10</v>
-      </c>
-      <c r="O3" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3">
-        <v>4.4000000000000004</v>
-      </c>
       <c r="Q3" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3" t="s">
+        <v>14</v>
+      </c>
+      <c r="T3" t="s">
+        <v>13</v>
+      </c>
+      <c r="U3">
         <v>1</v>
       </c>
-      <c r="T3" t="s">
-        <v>36</v>
-      </c>
-      <c r="U3">
-        <v>3</v>
-      </c>
       <c r="V3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3">
         <v>1</v>
@@ -1811,12 +1900,259 @@
       <c r="Y3">
         <v>0</v>
       </c>
-      <c r="Z3" t="s">
-        <v>17</v>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4">
+        <v>8765</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>3</v>
+      </c>
+      <c r="T4" t="s">
+        <v>33</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5">
+        <v>3646</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>7</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5" t="s">
+        <v>39</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T5" t="s">
+        <v>41</v>
+      </c>
+      <c r="U5">
+        <v>3</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2502</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6">
+        <v>6.5</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>40</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6" t="s">
+        <v>3</v>
+      </c>
+      <c r="T6" t="s">
+        <v>41</v>
+      </c>
+      <c r="U6">
+        <v>3</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:H5 I6:K6">
+  <conditionalFormatting sqref="A5:G5">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>"L1 = TRUE"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:K9 I8">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>"L1 = TRUE"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6:L6 J5">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>"L1 = TRUE"</formula>
     </cfRule>
@@ -1839,62 +2175,83 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2CD79F-6151-4C3C-A4EF-3143C630C872}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.265625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.1328125" customWidth="1"/>
+    <col min="8" max="8" width="22.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1">
-        <v>2134</v>
+        <v>246</v>
       </c>
       <c r="D1">
         <f>A1</f>
-        <v>2134</v>
+        <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <f>INDEX(Data!$L$2:$O$1000,MATCH(Sheet1!$D$1,Data!$F$2:$F$1000,0),MATCH(C2,Data!$L$1:$O$1,0))</f>
-        <v>3</v>
+        <v>59</v>
+      </c>
+      <c r="D2" t="e">
+        <f>INDEX(Data!$L$2:$O$1000,MATCH(IndividualTeam!$D$1,Data!$F$2:$F$1000,0),MATCH(C2,Data!$L$1:$O$1,0))</f>
+        <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3">
-        <f>INDEX(Data!$L$2:$O$1000,MATCH(Sheet1!$D$1,Data!$F$2:$F$1000,0),MATCH(C3,Data!$L$1:$O$1,0))</f>
-        <v>4</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D3" t="e">
+        <f>INDEX(Data!$L$2:$O$1000,MATCH(IndividualTeam!$D$1,Data!$F$2:$F$1000,0),MATCH(C3,Data!$L$1:$O$1,0))</f>
+        <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4">
-        <f>INDEX(Data!$L$2:$O$1000,MATCH(Sheet1!$D$1,Data!$F$2:$F$1000,0),MATCH(C4,Data!$L$1:$O$1,0))</f>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D4" t="e">
+        <f>INDEX(Data!$L$2:$O$1000,MATCH(IndividualTeam!$D$1,Data!$F$2:$F$1000,0),MATCH(C4,Data!$L$1:$O$1,0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D5" t="e">
+        <f>INDEX(Data!$L$2:$O$1000,MATCH(IndividualTeam!$D$1,Data!$F$2:$F$1000,0),MATCH(C5,Data!$L$1:$O$1,0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10">
+        <f>AVERAGE(MATCH($D$1,Data!$J$2:$J$1000))</f>
         <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="str">
-        <f>INDEX(Data!$L$2:$O$1000,MATCH(Sheet1!$D$1,Data!$F$2:$F$1000,0),MATCH(C5,Data!$L$1:$O$1,0))</f>
-        <v>b</v>
       </c>
     </row>
   </sheetData>

</xml_diff>